<commit_message>
update Sprintbacklog und diary
</commit_message>
<xml_diff>
--- a/doc/Task10/Product_Backlog.xlsx
+++ b/doc/Task10/Product_Backlog.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="80">
   <si>
     <t>ID</t>
   </si>
@@ -239,6 +239,42 @@
   </si>
   <si>
     <t>done</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Login </t>
+  </si>
+  <si>
+    <t>session</t>
+  </si>
+  <si>
+    <t>Patienten detailansicht</t>
+  </si>
+  <si>
+    <t>verbessern (Mobileansicht)</t>
+  </si>
+  <si>
+    <t>Refactoring code</t>
+  </si>
+  <si>
+    <t>alle</t>
+  </si>
+  <si>
+    <t>Comments, Benennung einheitlicht (English), allg. Konventionen</t>
+  </si>
+  <si>
+    <t>DB, UI</t>
+  </si>
+  <si>
+    <t>Findbugs</t>
+  </si>
+  <si>
+    <t>ausführen, resultat analysieren, gegebenenfalls korrigieren</t>
+  </si>
+  <si>
+    <t>Patienten suche</t>
+  </si>
+  <si>
+    <t>UI verbessern, Buttons direkt in der Tabelle</t>
   </si>
 </sst>
 </file>
@@ -689,8 +725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -748,7 +784,7 @@
         <v>47</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>7</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
@@ -788,7 +824,7 @@
         <v>9</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>7</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="117.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -848,7 +884,7 @@
         <v>9</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>7</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -873,10 +909,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1090,7 +1126,7 @@
         <v>4</v>
       </c>
       <c r="L6" t="s">
-        <v>7</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
@@ -1146,7 +1182,7 @@
         <v>16</v>
       </c>
       <c r="L8" t="s">
-        <v>7</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
@@ -1172,7 +1208,7 @@
         <v>2</v>
       </c>
       <c r="L9" t="s">
-        <v>7</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
@@ -1201,7 +1237,7 @@
         <v>4</v>
       </c>
       <c r="L10" t="s">
-        <v>7</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
@@ -1230,7 +1266,7 @@
         <v>3</v>
       </c>
       <c r="L11" t="s">
-        <v>7</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
@@ -1262,7 +1298,7 @@
         <v>7</v>
       </c>
       <c r="L12" t="s">
-        <v>7</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
@@ -1293,7 +1329,7 @@
         <v>2</v>
       </c>
       <c r="L13" t="s">
-        <v>7</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -1326,6 +1362,203 @@
         <v>6</v>
       </c>
       <c r="L14" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>4</v>
+      </c>
+      <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="F15" t="s">
+        <v>38</v>
+      </c>
+      <c r="G15" t="s">
+        <v>37</v>
+      </c>
+      <c r="H15" t="s">
+        <v>5</v>
+      </c>
+      <c r="I15">
+        <v>8</v>
+      </c>
+      <c r="L15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>5</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="F16" t="s">
+        <v>37</v>
+      </c>
+      <c r="G16" t="s">
+        <v>38</v>
+      </c>
+      <c r="H16" t="s">
+        <v>5</v>
+      </c>
+      <c r="I16">
+        <v>8</v>
+      </c>
+      <c r="L16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>6</v>
+      </c>
+      <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="C17" t="s">
+        <v>68</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F17" t="s">
+        <v>51</v>
+      </c>
+      <c r="G17" t="s">
+        <v>52</v>
+      </c>
+      <c r="H17" t="s">
+        <v>5</v>
+      </c>
+      <c r="I17">
+        <v>8</v>
+      </c>
+      <c r="L17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
+      </c>
+      <c r="C18" t="s">
+        <v>70</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="F18" t="s">
+        <v>52</v>
+      </c>
+      <c r="G18" t="s">
+        <v>51</v>
+      </c>
+      <c r="H18" t="s">
+        <v>5</v>
+      </c>
+      <c r="I18">
+        <v>6</v>
+      </c>
+      <c r="L18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B19">
+        <v>3</v>
+      </c>
+      <c r="C19" t="s">
+        <v>72</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="F19" t="s">
+        <v>73</v>
+      </c>
+      <c r="G19" t="s">
+        <v>73</v>
+      </c>
+      <c r="H19" t="s">
+        <v>5</v>
+      </c>
+      <c r="I19">
+        <v>2</v>
+      </c>
+      <c r="L19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B20">
+        <v>3</v>
+      </c>
+      <c r="C20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="F20" t="s">
+        <v>73</v>
+      </c>
+      <c r="G20" t="s">
+        <v>73</v>
+      </c>
+      <c r="H20" t="s">
+        <v>5</v>
+      </c>
+      <c r="I20">
+        <v>2</v>
+      </c>
+      <c r="L20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21">
+        <v>3</v>
+      </c>
+      <c r="C21" t="s">
+        <v>78</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="F21" t="s">
+        <v>52</v>
+      </c>
+      <c r="G21" t="s">
+        <v>51</v>
+      </c>
+      <c r="H21" t="s">
+        <v>5</v>
+      </c>
+      <c r="I21">
+        <v>2</v>
+      </c>
+      <c r="L21" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>